<commit_message>
create excel from fieldbook traits and plants added
</commit_message>
<xml_diff>
--- a/vavilov/test/data/observations1.xlsx
+++ b/vavilov/test/data/observations1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="12">
   <si>
     <t xml:space="preserve">assay</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha</t>
   </si>
   <si>
     <t xml:space="preserve">NSF1</t>
@@ -59,14 +62,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YYYY\ HH:MM:SS"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -94,6 +99,14 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF00AA00"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -140,7 +153,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -157,6 +170,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -166,6 +183,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF00AA00"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -174,19 +251,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.0102040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -208,19 +287,22 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>1</v>
@@ -228,19 +310,22 @@
       <c r="F2" s="0" t="n">
         <v>19</v>
       </c>
+      <c r="G2" s="4" t="n">
+        <v>42528.5654282407</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="0" t="n">
         <v>2</v>
@@ -248,19 +333,22 @@
       <c r="F3" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="G3" s="4" t="n">
+        <v>42528.5654282407</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>3</v>
@@ -268,19 +356,22 @@
       <c r="F4" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="G4" s="4" t="n">
+        <v>42528.5654282407</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>4</v>
@@ -288,19 +379,22 @@
       <c r="F5" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="G5" s="4" t="n">
+        <v>42528.5654282407</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>5</v>
@@ -308,19 +402,22 @@
       <c r="F6" s="0" t="n">
         <v>17</v>
       </c>
+      <c r="G6" s="4" t="n">
+        <v>42528.5654282407</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>1</v>
@@ -328,19 +425,22 @@
       <c r="F7" s="0" t="n">
         <v>19</v>
       </c>
+      <c r="G7" s="4" t="n">
+        <v>42528.5654282407</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>2</v>
@@ -348,19 +448,22 @@
       <c r="F8" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="G8" s="4" t="n">
+        <v>42528.5654282407</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>3</v>
@@ -368,19 +471,22 @@
       <c r="F9" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="G9" s="4" t="n">
+        <v>42528.5654282407</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E10" s="0" t="n">
         <v>4</v>
@@ -388,25 +494,31 @@
       <c r="F10" s="0" t="n">
         <v>18</v>
       </c>
+      <c r="G10" s="4" t="n">
+        <v>42528.5654282407</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E11" s="0" t="n">
         <v>5</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>17</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <v>42528.5654282407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
filter observations: new funtion and all filtering is made by this function
</commit_message>
<xml_diff>
--- a/vavilov/test/data/observations1.xlsx
+++ b/vavilov/test/data/observations1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="13">
   <si>
     <t xml:space="preserve">assay</t>
   </si>
@@ -56,6 +56,9 @@
   </si>
   <si>
     <t xml:space="preserve">BGV000928</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Growth habit</t>
   </si>
 </sst>
 </file>
@@ -251,21 +254,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G21" activeCellId="0" sqref="G21"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -519,6 +522,52 @@
       </c>
       <c r="G11" s="4" t="n">
         <v>42528.5654282407</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <v>42528.5661226852</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>2000</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <v>42528.5661226852</v>
       </c>
     </row>
   </sheetData>

</xml_diff>